<commit_message>
using pywin32 with current working directory
</commit_message>
<xml_diff>
--- a/Payroll/2012-01-01-Payroll.xlsx
+++ b/Payroll/2012-01-01-Payroll.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eraseme\examples\Payroll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\GitHub\examples\Payroll\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C1BC9B-00EA-4F0E-B69C-2D1399436119}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20175" windowHeight="9120"/>
+    <workbookView xWindow="6300" yWindow="1380" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAYROLL" sheetId="1" r:id="rId1"/>
@@ -85,16 +86,16 @@
     <t>From 1/01/2012 to 1/14/2012</t>
   </si>
   <si>
-    <t>JOHNSON, JEFF</t>
-  </si>
-  <si>
-    <t>SMITHFIELD, STEVE</t>
+    <t>DOE, JOHN</t>
+  </si>
+  <si>
+    <t>WALDRON, AUSTIN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
@@ -592,11 +593,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -969,7 +970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -981,7 +982,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>